<commit_message>
edited js along with backlog
</commit_message>
<xml_diff>
--- a/ProjectToDo/Backlog/Product_backlog_template.xlsx
+++ b/ProjectToDo/Backlog/Product_backlog_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IBA\WebSpecAssignments\tutorial project\webSpecTasks\ProjectToDo\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kenneth/Desktop/IBA/3semester/webSpecialization/webSpecTasks/ProjectToDo/Backlog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA5FEDF-8BFC-40AF-89D9-A8770DE240BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE12BA79-A74D-2E43-A463-A667DF6A5D9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="1620" windowWidth="21600" windowHeight="11385" xr2:uid="{1D807A5E-B5B4-C94B-9F79-296DA37239DA}"/>
+    <workbookView xWindow="5680" yWindow="1620" windowWidth="21600" windowHeight="11380" xr2:uid="{1D807A5E-B5B4-C94B-9F79-296DA37239DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>PRODUCT BACKLOG TEMPLATE</t>
   </si>
@@ -148,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -516,18 +516,18 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -546,7 +546,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -565,7 +565,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -588,7 +588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -605,7 +605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -622,7 +622,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -639,7 +639,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -656,7 +656,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="B8" t="s">
         <v>10</v>
       </c>
@@ -670,7 +670,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -684,7 +684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -698,7 +698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -712,7 +712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -726,7 +726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -740,7 +740,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -754,7 +754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -768,7 +768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -785,7 +785,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -797,6 +797,9 @@
       </c>
       <c r="E17">
         <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>